<commit_message>
add axis titles to physician 34 chart
</commit_message>
<xml_diff>
--- a/results/results_generated_conf_1.xlsx
+++ b/results/results_generated_conf_1.xlsx
@@ -1203,11 +1203,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-35561344"/>
-        <c:axId val="-35554272"/>
+        <c:axId val="-682386032"/>
+        <c:axId val="-682399632"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="-35554272"/>
+        <c:axId val="-682399632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1234,12 +1234,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-35561344"/>
+        <c:crossAx val="-682386032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-35561344"/>
+        <c:axId val="-682386032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1264,7 +1264,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-35554272"/>
+        <c:crossAx val="-682399632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2180,11 +2180,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-35559712"/>
-        <c:axId val="-35560800"/>
+        <c:axId val="-682394736"/>
+        <c:axId val="-682390928"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="-35560800"/>
+        <c:axId val="-682390928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2211,12 +2211,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-35559712"/>
+        <c:crossAx val="-682394736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-35559712"/>
+        <c:axId val="-682394736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2241,7 +2241,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-35560800"/>
+        <c:crossAx val="-682390928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2589,36 +2589,74 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-35558080"/>
-        <c:axId val="-35551008"/>
+        <c:axId val="-682392016"/>
+        <c:axId val="-682394192"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="-35551008"/>
+        <c:axId val="-682394192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" b="0"/>
+                  <a:t>satisfaction</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-35558080"/>
+        <c:crossAx val="-682392016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-35558080"/>
+        <c:axId val="-682392016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" b="0"/>
+                  <a:t>month</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-35551008"/>
+        <c:crossAx val="-682394192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -3022,9 +3060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF33" sqref="AF33"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>